<commit_message>
Update the results by major review
</commit_message>
<xml_diff>
--- a/Data/speedVs.xlsx
+++ b/Data/speedVs.xlsx
@@ -1,34 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\noav\Projects\Promo\Papier\InspectionProblem\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\noav\Projects\OptimizationOfImageAcquisition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C3144796-623F-4C45-BF8F-F88D33244D8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD58046D-8C51-4DD2-8B75-CE2181485248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="speed" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">speed!$B$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">speed!$B$2:$B$24</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">speed!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">speed!$C$2:$C$24</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">speed!$F$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">speed!$F$2:$F$24</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Geometrie</t>
   </si>
@@ -109,12 +114,27 @@
   </si>
   <si>
     <t>Rollout Monte-Carlo</t>
+  </si>
+  <si>
+    <t>Gridded Random</t>
+  </si>
+  <si>
+    <t>CAR_DOOR 1</t>
+  </si>
+  <si>
+    <t>CAR_DOOR 2</t>
+  </si>
+  <si>
+    <t>CAR_DOOR 3</t>
+  </si>
+  <si>
+    <t>CAR_DOOR 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -690,7 +710,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -705,64 +725,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>1002</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1002</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1000</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1004</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1002</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1003</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1004</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1005</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1000</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1004</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1007</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1002</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1014</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1009</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1006</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1012</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1003</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1015</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1014</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1002</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -804,64 +833,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>1001</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1001</c:v>
+                  <c:v>383</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1001</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1001</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1001</c:v>
+                  <c:v>6593</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1002</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1002</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1002</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1002</c:v>
+                  <c:v>398</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1003</c:v>
+                  <c:v>303</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1005</c:v>
+                  <c:v>3619</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1006</c:v>
+                  <c:v>4697</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1011</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1011</c:v>
+                  <c:v>19870</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1013</c:v>
+                  <c:v>1334</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1014</c:v>
+                  <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2002</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2023</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4033</c:v>
+                  <c:v>1992</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>18037</c:v>
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -903,64 +941,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>1013</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1007</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1007</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1015</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1014</c:v>
+                  <c:v>1303</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1003</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>300749</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1015</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1003</c:v>
+                  <c:v>20332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1006</c:v>
+                  <c:v>19683</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1009</c:v>
+                  <c:v>809</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>300380</c:v>
+                  <c:v>520</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1009</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1004</c:v>
+                  <c:v>2818</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1008</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1011</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1011</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1001</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1001</c:v>
+                  <c:v>294</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2019</c:v>
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,6 +1015,117 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-A536-4A67-A83A-511146526206}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>speed!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gridded Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>speed!$G$2:$G$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BF5-4BF5-8A4E-DB23BDE0991C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1037,7 +1195,7 @@
         <c:axId val="750186304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="18000"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1106,7 +1264,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.19097178477690291"/>
           <c:y val="0.89409667541557303"/>
-          <c:w val="0.54583398950131234"/>
+          <c:w val="0.78605643044619422"/>
           <c:h val="7.8125546806649182E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1732,16 +1890,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>528637</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>442911</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>223837</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2065,11 +2223,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,7 +2235,7 @@
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2097,472 +2255,627 @@
         <v>26</v>
       </c>
       <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>11</v>
       </c>
-      <c r="B2">
-        <v>1002</v>
-      </c>
-      <c r="C2">
-        <v>1001</v>
-      </c>
       <c r="D2">
-        <v>304307</v>
+        <v>121198</v>
       </c>
       <c r="E2">
-        <v>302652</v>
+        <v>111134</v>
       </c>
       <c r="F2">
-        <v>1013</v>
-      </c>
-      <c r="G2" s="1">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>23.000599999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>383</v>
+      </c>
+      <c r="D3">
+        <v>127073</v>
+      </c>
+      <c r="E3">
+        <v>72529</v>
+      </c>
+      <c r="F3">
+        <v>320</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1">
+        <v>104.74233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <v>126278</v>
+      </c>
+      <c r="E4">
+        <v>105365</v>
+      </c>
+      <c r="F4">
+        <v>66</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>14.154999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>129854</v>
+      </c>
+      <c r="E5">
+        <v>98654</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>43.933500000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <v>6593</v>
+      </c>
+      <c r="D6">
+        <v>115698</v>
+      </c>
+      <c r="E6">
+        <v>46530</v>
+      </c>
+      <c r="F6">
+        <v>1303</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>184.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>472</v>
+      </c>
+      <c r="D7">
+        <v>119287</v>
+      </c>
+      <c r="E7">
+        <v>50751</v>
+      </c>
+      <c r="F7">
+        <v>268</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>125514</v>
+      </c>
+      <c r="E8">
+        <v>102507</v>
+      </c>
+      <c r="F8">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>13.199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>103823</v>
+      </c>
+      <c r="E9">
+        <v>83993</v>
+      </c>
+      <c r="F9">
+        <v>70</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>398</v>
+      </c>
+      <c r="D10">
+        <v>111218</v>
+      </c>
+      <c r="E10">
+        <v>62690</v>
+      </c>
+      <c r="F10">
+        <v>20332</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>303</v>
+      </c>
+      <c r="D11">
+        <v>116670</v>
+      </c>
+      <c r="E11">
+        <v>68813</v>
+      </c>
+      <c r="F11">
+        <v>19683</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1">
+        <v>62.399000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>3619</v>
+      </c>
+      <c r="D12">
+        <v>107064</v>
+      </c>
+      <c r="E12">
+        <v>44264</v>
+      </c>
+      <c r="F12">
+        <v>809</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>4697</v>
+      </c>
+      <c r="D13">
+        <v>105714</v>
+      </c>
+      <c r="E13">
+        <v>31094</v>
+      </c>
+      <c r="F13">
+        <v>520</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>230</v>
+      </c>
+      <c r="D14">
+        <v>114129</v>
+      </c>
+      <c r="E14">
+        <v>64310</v>
+      </c>
+      <c r="F14">
+        <v>51</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>132</v>
+      </c>
+      <c r="C15">
+        <v>19870</v>
+      </c>
+      <c r="D15">
+        <v>92300</v>
+      </c>
+      <c r="E15">
+        <v>33565</v>
+      </c>
+      <c r="F15">
+        <v>2818</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>1334</v>
+      </c>
+      <c r="D16">
+        <v>112643</v>
+      </c>
+      <c r="E16">
+        <v>39642</v>
+      </c>
+      <c r="F16">
+        <v>248</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>401</v>
+      </c>
+      <c r="D17">
+        <v>109928</v>
+      </c>
+      <c r="E17">
+        <v>52239</v>
+      </c>
+      <c r="F17">
+        <v>110</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>46</v>
+      </c>
+      <c r="D18">
+        <v>121445</v>
+      </c>
+      <c r="E18">
+        <v>81637</v>
+      </c>
+      <c r="F18">
+        <v>51</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" s="1">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>103874</v>
+      </c>
+      <c r="E19">
+        <v>78910</v>
+      </c>
+      <c r="F19">
+        <v>39</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>1992</v>
+      </c>
+      <c r="D20">
+        <v>112016</v>
+      </c>
+      <c r="E20">
+        <v>46036</v>
+      </c>
+      <c r="F20">
+        <v>294</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20" s="1">
+        <v>62.399000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>55</v>
+      </c>
+      <c r="D21">
+        <v>113166</v>
+      </c>
+      <c r="E21">
+        <v>99188</v>
+      </c>
+      <c r="F21">
+        <v>108</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1">
         <v>7.5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3">
-        <v>1002</v>
-      </c>
-      <c r="C3">
-        <v>1001</v>
-      </c>
-      <c r="D3">
-        <v>304462</v>
-      </c>
-      <c r="E3">
-        <v>301913</v>
-      </c>
-      <c r="F3">
-        <v>1007</v>
-      </c>
-      <c r="G3" s="1">
-        <v>19.8</v>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>121265</v>
+      </c>
+      <c r="E22">
+        <v>96094</v>
+      </c>
+      <c r="F22">
+        <v>52</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
-        <v>1001</v>
-      </c>
-      <c r="D4">
-        <v>301202</v>
-      </c>
-      <c r="E4">
-        <v>301803</v>
-      </c>
-      <c r="F4">
-        <v>1007</v>
-      </c>
-      <c r="G4" s="1">
-        <v>25</v>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>132</v>
+      </c>
+      <c r="D23">
+        <v>113000</v>
+      </c>
+      <c r="E23">
+        <v>71783</v>
+      </c>
+      <c r="F23">
+        <v>80</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>1004</v>
-      </c>
-      <c r="C5">
-        <v>1001</v>
-      </c>
-      <c r="D5">
-        <v>303074</v>
-      </c>
-      <c r="E5">
-        <v>301966</v>
-      </c>
-      <c r="F5">
-        <v>1015</v>
-      </c>
-      <c r="G5" s="1">
-        <v>50</v>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>864</v>
+      </c>
+      <c r="D24">
+        <v>112869</v>
+      </c>
+      <c r="E24">
+        <v>46225</v>
+      </c>
+      <c r="F24">
+        <v>181</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6">
-        <v>1002</v>
-      </c>
-      <c r="C6">
-        <v>1001</v>
-      </c>
-      <c r="D6">
-        <v>306145</v>
-      </c>
-      <c r="E6">
-        <v>303734</v>
-      </c>
-      <c r="F6">
-        <v>1014</v>
-      </c>
-      <c r="G6" s="1">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>1003</v>
-      </c>
-      <c r="C7">
-        <v>1002</v>
-      </c>
-      <c r="D7">
-        <v>303835</v>
-      </c>
-      <c r="E7">
-        <v>300543</v>
-      </c>
-      <c r="F7">
-        <v>1003</v>
-      </c>
-      <c r="G7" s="1">
-        <v>43.933500000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>1004</v>
-      </c>
-      <c r="C8">
-        <v>1002</v>
-      </c>
-      <c r="D8">
-        <v>301873</v>
-      </c>
-      <c r="E8">
-        <v>302450</v>
-      </c>
-      <c r="F8">
-        <v>300749</v>
-      </c>
-      <c r="G8" s="1">
-        <v>62.399000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>1005</v>
-      </c>
-      <c r="C9">
-        <v>1002</v>
-      </c>
-      <c r="D9">
-        <v>301128</v>
-      </c>
-      <c r="E9">
-        <v>301705</v>
-      </c>
-      <c r="F9">
-        <v>1015</v>
-      </c>
-      <c r="G9" s="1">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10">
-        <v>1002</v>
-      </c>
-      <c r="D10">
-        <v>305310</v>
-      </c>
-      <c r="E10">
-        <v>303123</v>
-      </c>
-      <c r="F10">
-        <v>1003</v>
-      </c>
-      <c r="G10" s="1">
-        <v>104.74233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>1004</v>
-      </c>
-      <c r="C11">
-        <v>1003</v>
-      </c>
-      <c r="D11">
-        <v>304082</v>
-      </c>
-      <c r="E11">
-        <v>300966</v>
-      </c>
-      <c r="F11">
-        <v>1006</v>
-      </c>
-      <c r="G11" s="1">
-        <v>23.000599999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>1007</v>
-      </c>
-      <c r="C12">
-        <v>1005</v>
-      </c>
-      <c r="D12">
-        <v>302478</v>
-      </c>
-      <c r="E12">
-        <v>301848</v>
-      </c>
-      <c r="F12">
-        <v>1009</v>
-      </c>
-      <c r="G12" s="1">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>1002</v>
-      </c>
-      <c r="C13">
-        <v>1006</v>
-      </c>
-      <c r="D13">
-        <v>305555</v>
-      </c>
-      <c r="E13">
-        <v>302307</v>
-      </c>
-      <c r="F13">
-        <v>300380</v>
-      </c>
-      <c r="G13" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>1014</v>
-      </c>
-      <c r="C14">
-        <v>1011</v>
-      </c>
-      <c r="D14">
-        <v>306836</v>
-      </c>
-      <c r="E14">
-        <v>306456</v>
-      </c>
-      <c r="F14">
-        <v>1009</v>
-      </c>
-      <c r="G14" s="1">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>1009</v>
-      </c>
-      <c r="C15">
-        <v>1011</v>
-      </c>
-      <c r="D15">
-        <v>304292</v>
-      </c>
-      <c r="E15">
-        <v>302650</v>
-      </c>
-      <c r="F15">
-        <v>1004</v>
-      </c>
-      <c r="G15" s="1">
-        <v>14.154999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>1006</v>
-      </c>
-      <c r="C16">
-        <v>1013</v>
-      </c>
-      <c r="D16">
-        <v>302435</v>
-      </c>
-      <c r="E16">
-        <v>302227</v>
-      </c>
-      <c r="F16">
-        <v>1008</v>
-      </c>
-      <c r="G16" s="1">
-        <v>13.199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>1012</v>
-      </c>
-      <c r="C17">
-        <v>1014</v>
-      </c>
-      <c r="D17">
-        <v>303990</v>
-      </c>
-      <c r="E17">
-        <v>303323</v>
-      </c>
-      <c r="F17">
-        <v>1011</v>
-      </c>
-      <c r="G17" s="1">
-        <v>62.399000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18">
-        <v>1003</v>
-      </c>
-      <c r="C18">
-        <v>2002</v>
-      </c>
-      <c r="D18">
-        <v>303975</v>
-      </c>
-      <c r="E18">
-        <v>302056</v>
-      </c>
-      <c r="F18">
-        <v>1011</v>
-      </c>
-      <c r="G18" s="1">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19">
-        <v>1015</v>
-      </c>
-      <c r="C19">
-        <v>2023</v>
-      </c>
-      <c r="D19">
-        <v>304605</v>
-      </c>
-      <c r="E19">
-        <v>301839</v>
-      </c>
-      <c r="F19">
-        <v>1001</v>
-      </c>
-      <c r="G19" s="1">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>1014</v>
-      </c>
-      <c r="C20">
-        <v>4033</v>
-      </c>
-      <c r="D20">
-        <v>304269</v>
-      </c>
-      <c r="E20">
-        <v>302060</v>
-      </c>
-      <c r="F20">
-        <v>1001</v>
-      </c>
-      <c r="G20" s="1">
-        <v>184.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21">
-        <v>1002</v>
-      </c>
-      <c r="C21">
-        <v>18037</v>
-      </c>
-      <c r="D21">
-        <v>302658</v>
-      </c>
-      <c r="E21">
-        <v>300877</v>
-      </c>
-      <c r="F21">
-        <v>2019</v>
-      </c>
-      <c r="G21" s="1">
-        <v>25</v>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25">
+        <v>88</v>
+      </c>
+      <c r="C25">
+        <v>11169</v>
+      </c>
+      <c r="D25">
+        <v>94277</v>
+      </c>
+      <c r="E25">
+        <v>32940</v>
+      </c>
+      <c r="F25">
+        <v>2384</v>
+      </c>
+      <c r="G25">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G23">
-    <sortCondition ref="C1:C23"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G21">
+    <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update design of the diagrams
</commit_message>
<xml_diff>
--- a/Data/speedVs.xlsx
+++ b/Data/speedVs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\noav\Projects\OptimizationOfImageAcquisition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD58046D-8C51-4DD2-8B75-CE2181485248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7636D35-FAFF-47A7-8567-1C1B5DDC9A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -710,7 +710,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -803,224 +803,8 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>speed!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Greedy</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>speed!$C$2:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>383</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6593</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>472</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>398</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3619</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4697</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>230</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>19870</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1334</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>401</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1992</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>864</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A536-4A67-A83A-511146526206}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>speed!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Rollout Monte-Carlo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>speed!$F$2:$F$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>66</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1303</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>268</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>20332</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19683</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>809</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>520</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2818</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>294</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>181</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A536-4A67-A83A-511146526206}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>speed!$G$1</c:f>
@@ -1034,7 +818,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="7030A0"/>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1126,6 +912,238 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6BF5-4BF5-8A4E-DB23BDE0991C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>speed!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Greedy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="lgCheck">
+              <a:fgClr>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>speed!$C$2:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>383</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6593</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3619</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4697</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19870</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1334</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A536-4A67-A83A-511146526206}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>speed!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rollout Monte-Carlo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="lgGrid">
+              <a:fgClr>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>speed!$F$2:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20332</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19683</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>809</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2818</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>181</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A536-4A67-A83A-511146526206}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2227,7 +2245,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>